<commit_message>
pequenas alterações na tabela
</commit_message>
<xml_diff>
--- a/docs/exploratory_mine.xlsx
+++ b/docs/exploratory_mine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelef\Google Drive\2_profissional_krf\INMA\mineracao_bhrd\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D12918-01D7-407E-90E6-63E0CBDAAABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDEEFCA-8087-4873-B47B-74AFEB0FB8D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{AC7D7B23-30D3-4CDD-AC3A-7D383C57A9BE}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3085" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3065" uniqueCount="240">
   <si>
     <t>UPH_SG</t>
   </si>
@@ -750,60 +750,6 @@
     <t>UPH</t>
   </si>
   <si>
-    <t>0.036</t>
-  </si>
-  <si>
-    <t>0.428</t>
-  </si>
-  <si>
-    <t>0.077</t>
-  </si>
-  <si>
-    <t>0.088</t>
-  </si>
-  <si>
-    <t>0.626</t>
-  </si>
-  <si>
-    <t>0.054</t>
-  </si>
-  <si>
-    <t>0.564</t>
-  </si>
-  <si>
-    <t>0.039</t>
-  </si>
-  <si>
-    <t>0.448</t>
-  </si>
-  <si>
-    <t>0.016</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
-    <t>0.486</t>
-  </si>
-  <si>
-    <t>0.104</t>
-  </si>
-  <si>
-    <t>0.468</t>
-  </si>
-  <si>
-    <t>0.134</t>
-  </si>
-  <si>
-    <t>0.535</t>
-  </si>
-  <si>
-    <t>0.11</t>
-  </si>
-  <si>
-    <t>0.581</t>
-  </si>
-  <si>
     <t>Existente</t>
   </si>
   <si>
@@ -814,13 +760,16 @@
   </si>
   <si>
     <t>Disponível</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,6 +787,19 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -882,20 +844,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4435,11 +4412,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53C1247-3A46-4B1F-A87A-962F39F9F2F7}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E92"/>
+      <selection activeCell="G5" sqref="D5:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4471,47 +4447,47 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B2">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C2">
-        <v>193384673.462769</v>
+        <v>1385818.11108398</v>
       </c>
       <c r="D2">
-        <v>1.0999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B3">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C3">
-        <v>1341419.4296875</v>
+        <v>1192288.0175781201</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>181</v>
@@ -4519,19 +4495,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B4">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C4">
-        <v>1126413522.28528</v>
+        <v>133054015.397461</v>
       </c>
       <c r="D4">
-        <v>6.4000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>39</v>
@@ -4540,21 +4516,21 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B5">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C5">
-        <v>502399398.30358899</v>
+        <v>53788282.515869103</v>
       </c>
       <c r="D5">
-        <v>2.9000000000000001E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>47</v>
@@ -4563,21 +4539,21 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B6">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C6">
-        <v>56916299.161254898</v>
+        <v>23431566.050292999</v>
       </c>
       <c r="D6">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
         <v>37</v>
@@ -4586,21 +4562,21 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B7">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C7">
-        <v>28159018.498413101</v>
+        <v>16626443.0544434</v>
       </c>
       <c r="D7">
         <v>2E-3</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>43</v>
@@ -4609,21 +4585,21 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B8">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C8">
-        <v>19709800.267456099</v>
+        <v>14733512.5859375</v>
       </c>
       <c r="D8">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
         <v>47</v>
@@ -4632,21 +4608,21 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B9">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C9">
-        <v>9935662.63134766</v>
+        <v>7979596.5815429697</v>
       </c>
       <c r="D9">
         <v>1E-3</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
         <v>49</v>
@@ -4655,67 +4631,67 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B10">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C10">
-        <v>325030.48535156198</v>
+        <v>187149.48046875</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B11">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C11">
-        <v>196217.439819336</v>
+        <v>49024.237792968801</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B12">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C12">
-        <v>5211096582.8618202</v>
+        <v>1260698328.68115</v>
       </c>
       <c r="D12">
-        <v>0.29699999999999999</v>
+        <v>0.188</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
@@ -4724,21 +4700,21 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B13">
-        <v>17571415370.5303</v>
+        <v>6701355400.8986797</v>
       </c>
       <c r="C13">
-        <v>2301515439.6005902</v>
+        <v>212279189.832275</v>
       </c>
       <c r="D13">
-        <v>0.13100000000000001</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
         <v>52</v>
@@ -4747,21 +4723,21 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B14">
-        <v>5681533503.8906202</v>
+        <v>2483261754.22681</v>
       </c>
       <c r="C14">
-        <v>429833677.763794</v>
+        <v>66042641.941650398</v>
       </c>
       <c r="D14">
-        <v>7.5999999999999998E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
         <v>35</v>
@@ -4770,320 +4746,320 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B15">
-        <v>5681533503.8906202</v>
+        <v>2483261754.22681</v>
       </c>
       <c r="C15">
-        <v>5436094.1464843797</v>
+        <v>188393402.42236301</v>
       </c>
       <c r="D15">
-        <v>1E-3</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B16">
-        <v>5681533503.8906202</v>
+        <v>2483261754.22681</v>
       </c>
       <c r="C16">
-        <v>493815768.35192901</v>
+        <v>306689161.04467797</v>
       </c>
       <c r="D16">
-        <v>8.6999999999999994E-2</v>
+        <v>0.124</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B17">
-        <v>5681533503.8906202</v>
+        <v>2483261754.22681</v>
       </c>
       <c r="C17">
-        <v>418865776.74450701</v>
+        <v>20825906.665283199</v>
       </c>
       <c r="D17">
-        <v>7.3999999999999996E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B18">
-        <v>5681533503.8906202</v>
+        <v>2483261754.22681</v>
       </c>
       <c r="C18">
-        <v>40155635.611572303</v>
+        <v>6204174.41870117</v>
       </c>
       <c r="D18">
-        <v>7.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B19">
-        <v>5681533503.8906202</v>
+        <v>2483261754.22681</v>
       </c>
       <c r="C19">
-        <v>29919415.909179699</v>
+        <v>551205.21313476597</v>
       </c>
       <c r="D19">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B20">
-        <v>5681533503.8906202</v>
+        <v>2483261754.22681</v>
       </c>
       <c r="C20">
-        <v>6454903.4791259803</v>
+        <v>484606.99853515602</v>
       </c>
       <c r="D20">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B21">
-        <v>5681533503.8906202</v>
+        <v>2483261754.22681</v>
       </c>
       <c r="C21">
-        <v>4365082.6820068397</v>
+        <v>1260417219.80005</v>
       </c>
       <c r="D21">
-        <v>1E-3</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>508</v>
+      </c>
+      <c r="B22">
+        <v>2483261754.22681</v>
+      </c>
+      <c r="C22">
+        <v>65880425.245361298</v>
+      </c>
+      <c r="D22">
+        <v>2.7E-2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>506</v>
+      </c>
+      <c r="B23">
+        <v>9189326788.0202599</v>
+      </c>
+      <c r="C23">
+        <v>54202156.228515603</v>
+      </c>
+      <c r="D23">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>506</v>
+      </c>
+      <c r="B24">
+        <v>9189326788.0202599</v>
+      </c>
+      <c r="C24">
+        <v>471019.49438476597</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>506</v>
+      </c>
+      <c r="B25">
+        <v>9189326788.0202599</v>
+      </c>
+      <c r="C25">
+        <v>275880212.01611298</v>
+      </c>
+      <c r="D25">
+        <v>0.03</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>506</v>
+      </c>
+      <c r="B26">
+        <v>9189326788.0202599</v>
+      </c>
+      <c r="C26">
+        <v>633385693.90991199</v>
+      </c>
+      <c r="D26">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>502</v>
-      </c>
-      <c r="B22">
-        <v>5681533503.8906202</v>
-      </c>
-      <c r="C22">
-        <v>198941.788818359</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>502</v>
-      </c>
-      <c r="B23">
-        <v>5681533503.8906202</v>
-      </c>
-      <c r="C23">
-        <v>2568792995.2639198</v>
-      </c>
-      <c r="D23">
-        <v>0.45200000000000001</v>
-      </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>502</v>
-      </c>
-      <c r="B24">
-        <v>5681533503.8906202</v>
-      </c>
-      <c r="C24">
-        <v>988988926.75317395</v>
-      </c>
-      <c r="D24">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="E24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>503</v>
-      </c>
-      <c r="B25">
-        <v>10765433655.741699</v>
-      </c>
-      <c r="C25">
-        <v>254884816.00512701</v>
-      </c>
-      <c r="D25">
-        <v>2.4E-2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>503</v>
-      </c>
-      <c r="B26">
-        <v>10765433655.741699</v>
-      </c>
-      <c r="C26">
-        <v>4700348.6813964797</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B27">
-        <v>10765433655.741699</v>
+        <v>9189326788.0202599</v>
       </c>
       <c r="C27">
-        <v>885067204.96508801</v>
+        <v>156504934.69519001</v>
       </c>
       <c r="D27">
-        <v>8.2000000000000003E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B28">
-        <v>10765433655.741699</v>
+        <v>9189326788.0202599</v>
       </c>
       <c r="C28">
-        <v>493153787.73803699</v>
+        <v>19548745.287353501</v>
       </c>
       <c r="D28">
-        <v>4.5999999999999999E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F28" t="s">
         <v>47</v>
@@ -5092,44 +5068,44 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B29">
-        <v>10765433655.741699</v>
+        <v>9189326788.0202599</v>
       </c>
       <c r="C29">
-        <v>44605480.322265603</v>
+        <v>19242470.399658199</v>
       </c>
       <c r="D29">
-        <v>4.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F29" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B30">
-        <v>10765433655.741699</v>
+        <v>9189326788.0202599</v>
       </c>
       <c r="C30">
-        <v>24549737.509277299</v>
+        <v>6075680.22509766</v>
       </c>
       <c r="D30">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F30" t="s">
         <v>49</v>
@@ -5138,1240 +5114,1240 @@
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B31">
-        <v>10765433655.741699</v>
+        <v>9189326788.0202599</v>
       </c>
       <c r="C31">
-        <v>7419945.5043945303</v>
+        <v>13266.1032714844</v>
       </c>
       <c r="D31">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F31" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B32">
-        <v>10765433655.741699</v>
+        <v>9189326788.0202599</v>
       </c>
       <c r="C32">
-        <v>6465815.8771972703</v>
+        <v>3700028532.5117202</v>
       </c>
       <c r="D32">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>506</v>
+      </c>
+      <c r="B33">
+        <v>9189326788.0202599</v>
+      </c>
+      <c r="C33">
+        <v>758832689.24572802</v>
+      </c>
+      <c r="D33">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>502</v>
+      </c>
+      <c r="B34">
+        <v>5681533503.8906202</v>
+      </c>
+      <c r="C34">
+        <v>429833677.763794</v>
+      </c>
+      <c r="D34">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>502</v>
+      </c>
+      <c r="B35">
+        <v>5681533503.8906202</v>
+      </c>
+      <c r="C35">
+        <v>5436094.1464843797</v>
+      </c>
+      <c r="D35">
         <v>1E-3</v>
       </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>502</v>
+      </c>
+      <c r="B36">
+        <v>5681533503.8906202</v>
+      </c>
+      <c r="C36">
+        <v>493815768.35192901</v>
+      </c>
+      <c r="D36">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>502</v>
+      </c>
+      <c r="B37">
+        <v>5681533503.8906202</v>
+      </c>
+      <c r="C37">
+        <v>418865776.74450701</v>
+      </c>
+      <c r="D37">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" t="s">
         <v>47</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>503</v>
-      </c>
-      <c r="B33">
-        <v>10765433655.741699</v>
-      </c>
-      <c r="C33">
-        <v>297880.48364257801</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
-        <v>45</v>
-      </c>
-      <c r="G33" s="5" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>502</v>
+      </c>
+      <c r="B38">
+        <v>5681533503.8906202</v>
+      </c>
+      <c r="C38">
+        <v>40155635.611572303</v>
+      </c>
+      <c r="D38">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>503</v>
-      </c>
-      <c r="B34">
-        <v>10765433655.741699</v>
-      </c>
-      <c r="C34">
-        <v>179616.044677734</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" t="s">
-        <v>54</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>503</v>
-      </c>
-      <c r="B35">
-        <v>10765433655.741699</v>
-      </c>
-      <c r="C35">
-        <v>4495500605.6984901</v>
-      </c>
-      <c r="D35">
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="E35" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>503</v>
-      </c>
-      <c r="B36">
-        <v>10765433655.741699</v>
-      </c>
-      <c r="C36">
-        <v>1573108186.74683</v>
-      </c>
-      <c r="D36">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="E36" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" t="s">
-        <v>52</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>504</v>
-      </c>
-      <c r="B37">
-        <v>21557959763.5186</v>
-      </c>
-      <c r="C37">
-        <v>111477441.55590799</v>
-      </c>
-      <c r="D37">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E37" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" t="s">
-        <v>35</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>504</v>
-      </c>
-      <c r="B38">
-        <v>21557959763.5186</v>
-      </c>
-      <c r="C38">
-        <v>13133361.1086426</v>
-      </c>
-      <c r="D38">
-        <v>1E-3</v>
-      </c>
-      <c r="E38" t="s">
-        <v>22</v>
-      </c>
-      <c r="F38" t="s">
-        <v>41</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B39">
-        <v>21557959763.5186</v>
+        <v>5681533503.8906202</v>
       </c>
       <c r="C39">
-        <v>1221881887.9091799</v>
+        <v>29919415.909179699</v>
       </c>
       <c r="D39">
-        <v>5.7000000000000002E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E39" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B40">
-        <v>21557959763.5186</v>
+        <v>5681533503.8906202</v>
       </c>
       <c r="C40">
-        <v>655322700.36669898</v>
+        <v>6454903.4791259803</v>
       </c>
       <c r="D40">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="E40" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B41">
-        <v>21557959763.5186</v>
+        <v>5681533503.8906202</v>
       </c>
       <c r="C41">
-        <v>100004350.35913099</v>
+        <v>4365082.6820068397</v>
       </c>
       <c r="D41">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E41" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F41" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B42">
-        <v>21557959763.5186</v>
+        <v>5681533503.8906202</v>
       </c>
       <c r="C42">
-        <v>36991820.978271499</v>
+        <v>198941.788818359</v>
       </c>
       <c r="D42">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F42" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B43">
-        <v>21557959763.5186</v>
+        <v>5681533503.8906202</v>
       </c>
       <c r="C43">
-        <v>18455367.901367199</v>
+        <v>2568792995.2639198</v>
       </c>
       <c r="D43">
-        <v>1E-3</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="E43" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F43" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B44">
-        <v>21557959763.5186</v>
+        <v>5681533503.8906202</v>
       </c>
       <c r="C44">
-        <v>15054679.318115201</v>
+        <v>988988926.75317395</v>
       </c>
       <c r="D44">
-        <v>1E-3</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="E44" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F44" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B45">
-        <v>21557959763.5186</v>
+        <v>17571415370.5303</v>
       </c>
       <c r="C45">
-        <v>167100.078369141</v>
+        <v>193384673.462769</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E45" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F45" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B46">
-        <v>21557959763.5186</v>
+        <v>17571415370.5303</v>
       </c>
       <c r="C46">
-        <v>92148.9765625</v>
+        <v>1341419.4296875</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G46" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>501</v>
+      </c>
+      <c r="B47">
+        <v>17571415370.5303</v>
+      </c>
+      <c r="C47">
+        <v>1126413522.28528</v>
+      </c>
+      <c r="D47">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>501</v>
+      </c>
+      <c r="B48">
+        <v>17571415370.5303</v>
+      </c>
+      <c r="C48">
+        <v>502399398.30358899</v>
+      </c>
+      <c r="D48">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>504</v>
-      </c>
-      <c r="B47">
-        <v>21557959763.5186</v>
-      </c>
-      <c r="C47">
-        <v>8413343910.5720196</v>
-      </c>
-      <c r="D47">
-        <v>0.39</v>
-      </c>
-      <c r="E47" t="s">
-        <v>22</v>
-      </c>
-      <c r="F47" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>504</v>
-      </c>
-      <c r="B48">
-        <v>21557959763.5186</v>
-      </c>
-      <c r="C48">
-        <v>1254095790.98071</v>
-      </c>
-      <c r="D48">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="E48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F48" t="s">
-        <v>52</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B49">
-        <v>6701355400.8986797</v>
+        <v>17571415370.5303</v>
       </c>
       <c r="C49">
-        <v>1385818.11108398</v>
+        <v>56916299.161254898</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E49" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B50">
-        <v>6701355400.8986797</v>
+        <v>17571415370.5303</v>
       </c>
       <c r="C50">
-        <v>1192288.0175781201</v>
+        <v>28159018.498413101</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="E50" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F50" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B51">
-        <v>6701355400.8986797</v>
+        <v>17571415370.5303</v>
       </c>
       <c r="C51">
-        <v>133054015.397461</v>
+        <v>19709800.267456099</v>
       </c>
       <c r="D51">
-        <v>0.02</v>
+        <v>1E-3</v>
       </c>
       <c r="E51" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F51" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B52">
-        <v>6701355400.8986797</v>
+        <v>17571415370.5303</v>
       </c>
       <c r="C52">
-        <v>53788282.515869103</v>
+        <v>9935662.63134766</v>
       </c>
       <c r="D52">
-        <v>8.0000000000000002E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B53">
-        <v>6701355400.8986797</v>
+        <v>17571415370.5303</v>
       </c>
       <c r="C53">
-        <v>23431566.050292999</v>
+        <v>325030.48535156198</v>
       </c>
       <c r="D53">
-        <v>3.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F53" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B54">
-        <v>6701355400.8986797</v>
+        <v>17571415370.5303</v>
       </c>
       <c r="C54">
-        <v>16626443.0544434</v>
+        <v>196217.439819336</v>
       </c>
       <c r="D54">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F54" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B55">
-        <v>6701355400.8986797</v>
+        <v>17571415370.5303</v>
       </c>
       <c r="C55">
-        <v>14733512.5859375</v>
+        <v>5211096582.8618202</v>
       </c>
       <c r="D55">
-        <v>2E-3</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="E55" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F55" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>501</v>
+      </c>
+      <c r="B56">
+        <v>17571415370.5303</v>
+      </c>
+      <c r="C56">
+        <v>2301515439.6005902</v>
+      </c>
+      <c r="D56">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" t="s">
+        <v>52</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>507</v>
+      </c>
+      <c r="B57">
+        <v>9779833996.8535194</v>
+      </c>
+      <c r="C57">
+        <v>239068817.10620099</v>
+      </c>
+      <c r="D57">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>507</v>
+      </c>
+      <c r="B58">
+        <v>9779833996.8535194</v>
+      </c>
+      <c r="C58">
+        <v>585505302.75</v>
+      </c>
+      <c r="D58">
+        <v>0.06</v>
+      </c>
+      <c r="E58" t="s">
+        <v>31</v>
+      </c>
+      <c r="F58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>507</v>
+      </c>
+      <c r="B59">
+        <v>9779833996.8535194</v>
+      </c>
+      <c r="C59">
+        <v>887947780.6875</v>
+      </c>
+      <c r="D59">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" t="s">
         <v>47</v>
       </c>
-      <c r="G55" s="5" t="s">
+      <c r="G59" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>505</v>
-      </c>
-      <c r="B56">
-        <v>6701355400.8986797</v>
-      </c>
-      <c r="C56">
-        <v>7979596.5815429697</v>
-      </c>
-      <c r="D56">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>507</v>
+      </c>
+      <c r="B60">
+        <v>9779833996.8535194</v>
+      </c>
+      <c r="C60">
+        <v>73503567.291259795</v>
+      </c>
+      <c r="D60">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" t="s">
+        <v>37</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>507</v>
+      </c>
+      <c r="B61">
+        <v>9779833996.8535194</v>
+      </c>
+      <c r="C61">
+        <v>36873030.528564498</v>
+      </c>
+      <c r="D61">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>31</v>
+      </c>
+      <c r="F61" t="s">
+        <v>43</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>507</v>
+      </c>
+      <c r="B62">
+        <v>9779833996.8535194</v>
+      </c>
+      <c r="C62">
+        <v>11150284.916748</v>
+      </c>
+      <c r="D62">
         <v>1E-3</v>
       </c>
-      <c r="E56" t="s">
-        <v>25</v>
-      </c>
-      <c r="F56" t="s">
-        <v>49</v>
-      </c>
-      <c r="G56" s="5" t="s">
+      <c r="E62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" t="s">
+        <v>47</v>
+      </c>
+      <c r="G62" s="5" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>505</v>
-      </c>
-      <c r="B57">
-        <v>6701355400.8986797</v>
-      </c>
-      <c r="C57">
-        <v>187149.48046875</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57" t="s">
-        <v>25</v>
-      </c>
-      <c r="F57" t="s">
-        <v>54</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>505</v>
-      </c>
-      <c r="B58">
-        <v>6701355400.8986797</v>
-      </c>
-      <c r="C58">
-        <v>49024.237792968801</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58" t="s">
-        <v>25</v>
-      </c>
-      <c r="F58" t="s">
-        <v>45</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>505</v>
-      </c>
-      <c r="B59">
-        <v>6701355400.8986797</v>
-      </c>
-      <c r="C59">
-        <v>1260698328.68115</v>
-      </c>
-      <c r="D59">
-        <v>0.188</v>
-      </c>
-      <c r="E59" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" t="s">
-        <v>13</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>505</v>
-      </c>
-      <c r="B60">
-        <v>6701355400.8986797</v>
-      </c>
-      <c r="C60">
-        <v>212279189.832275</v>
-      </c>
-      <c r="D60">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="E60" t="s">
-        <v>25</v>
-      </c>
-      <c r="F60" t="s">
-        <v>52</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>506</v>
-      </c>
-      <c r="B61">
-        <v>9189326788.0202599</v>
-      </c>
-      <c r="C61">
-        <v>54202156.228515603</v>
-      </c>
-      <c r="D61">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="E61" t="s">
-        <v>28</v>
-      </c>
-      <c r="F61" t="s">
-        <v>35</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>506</v>
-      </c>
-      <c r="B62">
-        <v>9189326788.0202599</v>
-      </c>
-      <c r="C62">
-        <v>471019.49438476597</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62" t="s">
-        <v>28</v>
-      </c>
-      <c r="F62" t="s">
-        <v>41</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B63">
-        <v>9189326788.0202599</v>
+        <v>9779833996.8535194</v>
       </c>
       <c r="C63">
-        <v>275880212.01611298</v>
+        <v>2094138.53051758</v>
       </c>
       <c r="D63">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F63" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B64">
-        <v>9189326788.0202599</v>
+        <v>9779833996.8535194</v>
       </c>
       <c r="C64">
-        <v>633385693.90991199</v>
+        <v>50002.510253906199</v>
       </c>
       <c r="D64">
-        <v>6.9000000000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F64" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B65">
-        <v>9189326788.0202599</v>
+        <v>9779833996.8535194</v>
       </c>
       <c r="C65">
-        <v>156504934.69519001</v>
+        <v>4233779632.6572299</v>
       </c>
       <c r="D65">
-        <v>1.7000000000000001E-2</v>
+        <v>0.433</v>
       </c>
       <c r="E65" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F65" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B66">
-        <v>9189326788.0202599</v>
+        <v>9779833996.8535194</v>
       </c>
       <c r="C66">
-        <v>19548745.287353501</v>
+        <v>346760506.67358398</v>
       </c>
       <c r="D66">
-        <v>2E-3</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E66" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F66" t="s">
+        <v>52</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>509</v>
+      </c>
+      <c r="B67">
+        <v>2825810954.6467299</v>
+      </c>
+      <c r="C67">
+        <v>82031872.286132798</v>
+      </c>
+      <c r="D67">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E67" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67" t="s">
+        <v>35</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>509</v>
+      </c>
+      <c r="B68">
+        <v>2825810954.6467299</v>
+      </c>
+      <c r="C68">
+        <v>124691047.432861</v>
+      </c>
+      <c r="D68">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>33</v>
+      </c>
+      <c r="F68" t="s">
+        <v>39</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>509</v>
+      </c>
+      <c r="B69">
+        <v>2825810954.6467299</v>
+      </c>
+      <c r="C69">
+        <v>297674507.70947301</v>
+      </c>
+      <c r="D69">
+        <v>0.105</v>
+      </c>
+      <c r="E69" t="s">
+        <v>33</v>
+      </c>
+      <c r="F69" t="s">
         <v>47</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>506</v>
-      </c>
-      <c r="B67">
-        <v>9189326788.0202599</v>
-      </c>
-      <c r="C67">
-        <v>19242470.399658199</v>
-      </c>
-      <c r="D67">
-        <v>2E-3</v>
-      </c>
-      <c r="E67" t="s">
-        <v>28</v>
-      </c>
-      <c r="F67" t="s">
-        <v>43</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>506</v>
-      </c>
-      <c r="B68">
-        <v>9189326788.0202599</v>
-      </c>
-      <c r="C68">
-        <v>6075680.22509766</v>
-      </c>
-      <c r="D68">
-        <v>1E-3</v>
-      </c>
-      <c r="E68" t="s">
-        <v>28</v>
-      </c>
-      <c r="F68" t="s">
-        <v>49</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>506</v>
-      </c>
-      <c r="B69">
-        <v>9189326788.0202599</v>
-      </c>
-      <c r="C69">
-        <v>13266.1032714844</v>
-      </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69" t="s">
-        <v>28</v>
-      </c>
-      <c r="F69" t="s">
-        <v>54</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="B70">
-        <v>9189326788.0202599</v>
+        <v>2825810954.6467299</v>
       </c>
       <c r="C70">
-        <v>3700028532.5117202</v>
+        <v>6820154.99755859</v>
       </c>
       <c r="D70">
-        <v>0.40300000000000002</v>
+        <v>2E-3</v>
       </c>
       <c r="E70" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F70" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="B71">
-        <v>9189326788.0202599</v>
+        <v>2825810954.6467299</v>
       </c>
       <c r="C71">
-        <v>758832689.24572802</v>
+        <v>5279256.1025390597</v>
       </c>
       <c r="D71">
-        <v>8.3000000000000004E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E71" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F71" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B72">
-        <v>9779833996.8535194</v>
+        <v>2825810954.6467299</v>
       </c>
       <c r="C72">
-        <v>239068817.10620099</v>
+        <v>1977060.42822266</v>
       </c>
       <c r="D72">
-        <v>2.4E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="E72" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F72" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B73">
-        <v>9779833996.8535194</v>
+        <v>2825810954.6467299</v>
       </c>
       <c r="C73">
-        <v>585505302.75</v>
+        <v>500022.697265625</v>
       </c>
       <c r="D73">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F73" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B74">
-        <v>9779833996.8535194</v>
+        <v>2825810954.6467299</v>
       </c>
       <c r="C74">
-        <v>887947780.6875</v>
+        <v>78540.3876953125</v>
       </c>
       <c r="D74">
-        <v>9.0999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F74" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B75">
-        <v>9779833996.8535194</v>
+        <v>2825810954.6467299</v>
       </c>
       <c r="C75">
-        <v>73503567.291259795</v>
+        <v>1602145121.4223599</v>
       </c>
       <c r="D75">
-        <v>8.0000000000000002E-3</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="E75" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F75" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B76">
-        <v>9779833996.8535194</v>
+        <v>2825810954.6467299</v>
       </c>
       <c r="C76">
-        <v>36873030.528564498</v>
+        <v>38978005.4365234</v>
       </c>
       <c r="D76">
-        <v>4.0000000000000001E-3</v>
+        <v>1.4E-2</v>
       </c>
       <c r="E76" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F76" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B77">
-        <v>9779833996.8535194</v>
+        <v>10765433655.741699</v>
       </c>
       <c r="C77">
-        <v>11150284.916748</v>
+        <v>254884816.00512701</v>
       </c>
       <c r="D77">
-        <v>1E-3</v>
+        <v>2.4E-2</v>
       </c>
       <c r="E77" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B78">
-        <v>9779833996.8535194</v>
+        <v>10765433655.741699</v>
       </c>
       <c r="C78">
-        <v>2094138.53051758</v>
+        <v>4700348.6813964797</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F78" t="s">
+        <v>41</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>503</v>
+      </c>
+      <c r="B79">
+        <v>10765433655.741699</v>
+      </c>
+      <c r="C79">
+        <v>885067204.96508801</v>
+      </c>
+      <c r="D79">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E79" t="s">
+        <v>19</v>
+      </c>
+      <c r="F79" t="s">
+        <v>39</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>503</v>
+      </c>
+      <c r="B80">
+        <v>10765433655.741699</v>
+      </c>
+      <c r="C80">
+        <v>493153787.73803699</v>
+      </c>
+      <c r="D80">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E80" t="s">
+        <v>19</v>
+      </c>
+      <c r="F80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>503</v>
+      </c>
+      <c r="B81">
+        <v>10765433655.741699</v>
+      </c>
+      <c r="C81">
+        <v>44605480.322265603</v>
+      </c>
+      <c r="D81">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E81" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" t="s">
+        <v>37</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>503</v>
+      </c>
+      <c r="B82">
+        <v>10765433655.741699</v>
+      </c>
+      <c r="C82">
+        <v>24549737.509277299</v>
+      </c>
+      <c r="D82">
+        <v>2E-3</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
         <v>49</v>
       </c>
-      <c r="G78" s="5" t="s">
+      <c r="G82" s="5" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>507</v>
-      </c>
-      <c r="B79">
-        <v>9779833996.8535194</v>
-      </c>
-      <c r="C79">
-        <v>50002.510253906199</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79" t="s">
-        <v>31</v>
-      </c>
-      <c r="F79" t="s">
-        <v>54</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>507</v>
-      </c>
-      <c r="B80">
-        <v>9779833996.8535194</v>
-      </c>
-      <c r="C80">
-        <v>4233779632.6572299</v>
-      </c>
-      <c r="D80">
-        <v>0.433</v>
-      </c>
-      <c r="E80" t="s">
-        <v>31</v>
-      </c>
-      <c r="F80" t="s">
-        <v>13</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>507</v>
-      </c>
-      <c r="B81">
-        <v>9779833996.8535194</v>
-      </c>
-      <c r="C81">
-        <v>346760506.67358398</v>
-      </c>
-      <c r="D81">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="E81" t="s">
-        <v>31</v>
-      </c>
-      <c r="F81" t="s">
-        <v>52</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>508</v>
-      </c>
-      <c r="B82">
-        <v>2483261754.22681</v>
-      </c>
-      <c r="C82">
-        <v>66042641.941650398</v>
-      </c>
-      <c r="D82">
-        <v>2.7E-2</v>
-      </c>
-      <c r="E82" t="s">
-        <v>32</v>
-      </c>
-      <c r="F82" t="s">
-        <v>35</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B83">
-        <v>2483261754.22681</v>
+        <v>10765433655.741699</v>
       </c>
       <c r="C83">
-        <v>188393402.42236301</v>
+        <v>7419945.5043945303</v>
       </c>
       <c r="D83">
-        <v>7.5999999999999998E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="E83" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B84">
-        <v>2483261754.22681</v>
+        <v>10765433655.741699</v>
       </c>
       <c r="C84">
-        <v>306689161.04467797</v>
+        <v>6465815.8771972703</v>
       </c>
       <c r="D84">
-        <v>0.124</v>
+        <v>1E-3</v>
       </c>
       <c r="E84" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F84" t="s">
         <v>47</v>
@@ -6380,320 +6356,320 @@
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B85">
-        <v>2483261754.22681</v>
+        <v>10765433655.741699</v>
       </c>
       <c r="C85">
-        <v>20825906.665283199</v>
+        <v>297880.48364257801</v>
       </c>
       <c r="D85">
-        <v>8.0000000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F85" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B86">
-        <v>2483261754.22681</v>
+        <v>10765433655.741699</v>
       </c>
       <c r="C86">
-        <v>6204174.41870117</v>
+        <v>179616.044677734</v>
       </c>
       <c r="D86">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B87">
-        <v>2483261754.22681</v>
+        <v>10765433655.741699</v>
       </c>
       <c r="C87">
-        <v>551205.21313476597</v>
+        <v>4495500605.6984901</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="E87" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B88">
-        <v>2483261754.22681</v>
+        <v>10765433655.741699</v>
       </c>
       <c r="C88">
-        <v>484606.99853515602</v>
+        <v>1573108186.74683</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="E88" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B89">
-        <v>2483261754.22681</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C89">
-        <v>1260417219.80005</v>
+        <v>111477441.55590799</v>
       </c>
       <c r="D89">
-        <v>0.50800000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E89" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F89" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B90">
-        <v>2483261754.22681</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C90">
-        <v>65880425.245361298</v>
+        <v>13133361.1086426</v>
       </c>
       <c r="D90">
-        <v>2.7E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="E90" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F90" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B91">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C91">
-        <v>82031872.286132798</v>
+        <v>1221881887.9091799</v>
       </c>
       <c r="D91">
-        <v>2.9000000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="E91" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F91" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B92">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C92">
-        <v>124691047.432861</v>
+        <v>655322700.36669898</v>
       </c>
       <c r="D92">
-        <v>4.3999999999999997E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E92" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F92" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B93">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C93">
-        <v>297674507.70947301</v>
+        <v>100004350.35913099</v>
       </c>
       <c r="D93">
-        <v>0.105</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E93" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F93" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B94">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C94">
-        <v>6820154.99755859</v>
+        <v>36991820.978271499</v>
       </c>
       <c r="D94">
         <v>2E-3</v>
       </c>
       <c r="E94" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F94" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B95">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C95">
-        <v>5279256.1025390597</v>
+        <v>18455367.901367199</v>
       </c>
       <c r="D95">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E95" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F95" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B96">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C96">
-        <v>1977060.42822266</v>
+        <v>15054679.318115201</v>
       </c>
       <c r="D96">
         <v>1E-3</v>
       </c>
       <c r="E96" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F96" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B97">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C97">
-        <v>500022.697265625</v>
+        <v>167100.078369141</v>
       </c>
       <c r="D97">
         <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F97" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G97" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B98">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C98">
-        <v>78540.3876953125</v>
+        <v>92148.9765625</v>
       </c>
       <c r="D98">
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F98" t="s">
         <v>45</v>
@@ -6702,21 +6678,21 @@
         <v>182</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B99">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C99">
-        <v>1602145121.4223599</v>
+        <v>8413343910.5720196</v>
       </c>
       <c r="D99">
-        <v>0.56699999999999995</v>
+        <v>0.39</v>
       </c>
       <c r="E99" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F99" t="s">
         <v>13</v>
@@ -6725,21 +6701,21 @@
         <v>180</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B100">
-        <v>2825810954.6467299</v>
+        <v>21557959763.5186</v>
       </c>
       <c r="C100">
-        <v>38978005.4365234</v>
+        <v>1254095790.98071</v>
       </c>
       <c r="D100">
-        <v>1.4E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="E100" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F100" t="s">
         <v>52</v>
@@ -6750,11 +6726,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G100" xr:uid="{847D609D-7D14-445D-B520-A9C5F074201A}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="NA"/>
-      </filters>
-    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G100">
+      <sortCondition ref="E2:E100"/>
+      <sortCondition ref="G2:G100"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -6762,188 +6737,422 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0388BD46-B007-464E-AFEE-87DD40B0A906}">
-  <dimension ref="G2:K11"/>
+  <dimension ref="G2:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:K11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="9.140625" style="7"/>
+    <col min="7" max="7" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="7"/>
+    <col min="11" max="11" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="7"/>
+    <col min="13" max="13" width="21.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G2" s="7" t="s">
+    <row r="2" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G2" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G3" t="s">
+      <c r="H2" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="K3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G4" t="s">
+      <c r="H3" s="8">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I3" s="8">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="K3" s="7">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="11">
+        <f>H3*100</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="O3" s="11">
+        <f t="shared" ref="O3:Q3" si="0">I3*100</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="P3" s="11">
+        <f t="shared" si="0"/>
+        <v>42.8</v>
+      </c>
+      <c r="Q3" s="11">
+        <f t="shared" si="0"/>
+        <v>6.4</v>
+      </c>
+      <c r="R3" s="11">
+        <f>SUM(N3:Q3)</f>
+        <v>53.9</v>
+      </c>
+    </row>
+    <row r="4" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="K4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G5" t="s">
+      <c r="H4" s="8">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="I4" s="8">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.626</v>
+      </c>
+      <c r="K4" s="7">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="14">
+        <f t="shared" ref="N4:N11" si="1">H4*100</f>
+        <v>7.7</v>
+      </c>
+      <c r="O4" s="14">
+        <f t="shared" ref="O4:O11" si="2">I4*100</f>
+        <v>8.7999999999999989</v>
+      </c>
+      <c r="P4" s="14">
+        <f t="shared" ref="P4:P11" si="3">J4*100</f>
+        <v>62.6</v>
+      </c>
+      <c r="Q4" s="14">
+        <f t="shared" ref="Q4:Q11" si="4">K4*100</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="R4" s="14">
+        <f t="shared" ref="R4:R11" si="5">SUM(N4:Q4)</f>
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="5" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="K5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G6" t="s">
+      <c r="H5" s="8">
+        <v>2.4E-2</v>
+      </c>
+      <c r="I5" s="8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="K5" s="7">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="14">
+        <f t="shared" si="1"/>
+        <v>2.4</v>
+      </c>
+      <c r="O5" s="14">
+        <f t="shared" si="2"/>
+        <v>5.4</v>
+      </c>
+      <c r="P5" s="14">
+        <f t="shared" si="3"/>
+        <v>56.399999999999991</v>
+      </c>
+      <c r="Q5" s="14">
+        <f t="shared" si="4"/>
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="R5" s="14">
+        <f t="shared" si="5"/>
+        <v>72.399999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G6" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="K6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
+      <c r="H6" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I6" s="8">
+        <v>3.9E-2</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="K6" s="7">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="O6" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9</v>
+      </c>
+      <c r="P6" s="11">
+        <f t="shared" si="3"/>
+        <v>44.800000000000004</v>
+      </c>
+      <c r="Q6" s="11">
+        <f t="shared" si="4"/>
+        <v>5.7</v>
+      </c>
+      <c r="R6" s="11">
+        <f t="shared" si="5"/>
+        <v>55.000000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="8">
         <v>0</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="K7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
+      <c r="I7" s="8">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="11">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+      <c r="P7" s="11">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="R7" s="11">
+        <f t="shared" si="5"/>
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="8" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G8" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="K8" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="9" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
+      <c r="H8" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I8" s="8">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="O8" s="11">
+        <f t="shared" si="2"/>
+        <v>9.1</v>
+      </c>
+      <c r="P8" s="11">
+        <f t="shared" si="3"/>
+        <v>48.6</v>
+      </c>
+      <c r="Q8" s="11">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="R8" s="11">
+        <f t="shared" si="5"/>
+        <v>61.3</v>
+      </c>
+    </row>
+    <row r="9" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G9" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="K9" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="10" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
+      <c r="H9" s="8">
+        <v>2.4E-2</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.104</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="1"/>
+        <v>2.4</v>
+      </c>
+      <c r="O9" s="11">
+        <f t="shared" si="2"/>
+        <v>10.4</v>
+      </c>
+      <c r="P9" s="11">
+        <f t="shared" si="3"/>
+        <v>46.800000000000004</v>
+      </c>
+      <c r="Q9" s="11">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="R9" s="11">
+        <f t="shared" si="5"/>
+        <v>65.600000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="K10" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G11" s="8" t="s">
+      <c r="H10" s="8">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="K10" s="7">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="14">
+        <f t="shared" si="1"/>
+        <v>2.7</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="2"/>
+        <v>13.4</v>
+      </c>
+      <c r="P10" s="14">
+        <f t="shared" si="3"/>
+        <v>53.5</v>
+      </c>
+      <c r="Q10" s="14">
+        <f t="shared" si="4"/>
+        <v>7.6</v>
+      </c>
+      <c r="R10" s="14">
+        <f t="shared" si="5"/>
+        <v>77.199999999999989</v>
+      </c>
+    </row>
+    <row r="11" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G11" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>226</v>
+      <c r="H11" s="10">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="K11" s="9">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="N11" s="16">
+        <f t="shared" si="1"/>
+        <v>2.9000000000000004</v>
+      </c>
+      <c r="O11" s="16">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="P11" s="16">
+        <f t="shared" si="3"/>
+        <v>58.099999999999994</v>
+      </c>
+      <c r="Q11" s="16">
+        <f t="shared" si="4"/>
+        <v>4.3999999999999995</v>
+      </c>
+      <c r="R11" s="16">
+        <f t="shared" si="5"/>
+        <v>76.400000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>